<commit_message>
fix keyboard kill for registry
</commit_message>
<xml_diff>
--- a/tests/sourcegen.xlsx
+++ b/tests/sourcegen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenrees/PycharmProjects/CS6381/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DC343B-77FB-3E4B-8376-AFBA18D714EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C144F425-5576-AE43-930F-22C6E447DE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2500" windowWidth="27240" windowHeight="16440" xr2:uid="{3BD69431-E4D0-FC4E-B40B-EBF74BC55B51}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,19 +505,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>4</v>
@@ -571,8 +571,8 @@
         <v>h1x1</v>
       </c>
       <c r="F3" t="str">
-        <f>IF($A3="","",_xlfn.CONCAT(E3," python3 -u ",$B3,IF(AND($A3=1,$B$1&gt;0)," -d broker",""),IF($B3=$G$1,_xlfn.CONCAT(" -c ",$D$1," -s ",$F$1),"")," -r 10.0.0.1 &amp;&gt; ",$E3,".out &amp;"))</f>
-        <v>h1x1 python3 -u registryapp.py -d broker -c 49 -s 49 -r 10.0.0.1 &amp;&gt; h1x1.out &amp;</v>
+        <f ca="1">IF($A3="","",_xlfn.CONCAT(E3," python3 -u ",$B3,IF(AND(B3=$G$1,$B$1&gt;0)," -d broker",""),IF(B3=$G$1,IF(A3=1,"",_xlfn.CONCAT(" -n ",A3-1)),_xlfn.CONCAT(" -r 10.0.0.",IF(OR(B3=$A$1,B3=$E$1),RANDBETWEEN(1,$H$1),1))),IF(OR(B3=$A$1,B3=$E$1),_xlfn.CONCAT(" -n ",$H$1),"")," &amp;&gt; ",$E3,".out &amp;"))</f>
+        <v>h1x1 python3 -u registryapp.py -d broker &amp;&gt; h1x1.out &amp;</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -582,7 +582,7 @@
       </c>
       <c r="B4" t="str">
         <f>IF(COUNTIF($B$2:$B3,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B3,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B3,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B3,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>brokerapp.py</v>
+        <v>registryapp.py</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -597,8 +597,8 @@
         <v>h1x2</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F67" si="4">IF($A4="","",_xlfn.CONCAT(E4," python3 -u ",$B4,IF(AND($A4=1,$B$1&gt;0)," -d broker",""),IF($B4=$G$1,_xlfn.CONCAT(" -c ",$D$1," -s ",$F$1),"")," -r 10.0.0.1 &amp;&gt; ",$E4,".out &amp;"))</f>
-        <v>h1x2 python3 -u brokerapp.py -r 10.0.0.1 &amp;&gt; h1x2.out &amp;</v>
+        <f t="shared" ref="F4:F67" ca="1" si="4">IF($A4="","",_xlfn.CONCAT(E4," python3 -u ",$B4,IF(AND(B4=$G$1,$B$1&gt;0)," -d broker",""),IF(B4=$G$1,IF(A4=1,"",_xlfn.CONCAT(" -n ",A4-1)),_xlfn.CONCAT(" -r 10.0.0.",IF(OR(B4=$A$1,B4=$E$1),RANDBETWEEN(1,$H$1),1))),IF(OR(B4=$A$1,B4=$E$1),_xlfn.CONCAT(" -n ",$H$1),"")," &amp;&gt; ",$E4,".out &amp;"))</f>
+        <v>h1x2 python3 -u registryapp.py -d broker -n 1 &amp;&gt; h1x2.out &amp;</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -608,7 +608,7 @@
       </c>
       <c r="B5" t="str">
         <f>IF(COUNTIF($B$2:$B4,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B4,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B4,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B4,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>registryapp.py</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -623,8 +623,8 @@
         <v>h1x3</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="4"/>
-        <v>h1x3 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h1x3.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h1x3 python3 -u registryapp.py -d broker -n 2 &amp;&gt; h1x3.out &amp;</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -634,7 +634,7 @@
       </c>
       <c r="B6" t="str">
         <f>IF(COUNTIF($B$2:$B5,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B5,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B5,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B5,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>registryapp.py</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -649,8 +649,8 @@
         <v>h1x4</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="4"/>
-        <v>h1x4 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h1x4.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h1x4 python3 -u registryapp.py -d broker -n 3 &amp;&gt; h1x4.out &amp;</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
       </c>
       <c r="B7" t="str">
         <f>IF(COUNTIF($B$2:$B6,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B6,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B6,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B6,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>registryapp.py</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -675,8 +675,8 @@
         <v>h1x5</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="4"/>
-        <v>h1x5 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h1x5.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h1x5 python3 -u registryapp.py -d broker -n 4 &amp;&gt; h1x5.out &amp;</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
       </c>
       <c r="B8" t="str">
         <f>IF(COUNTIF($B$2:$B7,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B7,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B7,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B7,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>registryapp.py</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -701,8 +701,8 @@
         <v>h1x6</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="4"/>
-        <v>h1x6 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h1x6.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h1x6 python3 -u registryapp.py -d broker -n 5 &amp;&gt; h1x6.out &amp;</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -712,7 +712,7 @@
       </c>
       <c r="B9" t="str">
         <f>IF(COUNTIF($B$2:$B8,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B8,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B8,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B8,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>registryapp.py</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -727,8 +727,8 @@
         <v>h1x7</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="4"/>
-        <v>h1x7 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h1x7.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h1x7 python3 -u registryapp.py -d broker -n 6 &amp;&gt; h1x7.out &amp;</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
       </c>
       <c r="B10" t="str">
         <f>IF(COUNTIF($B$2:$B9,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B9,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B9,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B9,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>registryapp.py</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -753,8 +753,8 @@
         <v>h1x8</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="4"/>
-        <v>h1x8 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h1x8.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h1x8 python3 -u registryapp.py -d broker -n 7 &amp;&gt; h1x8.out &amp;</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -764,7 +764,7 @@
       </c>
       <c r="B11" t="str">
         <f>IF(COUNTIF($B$2:$B10,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B10,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B10,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B10,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>registryapp.py</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -779,8 +779,8 @@
         <v>h1x9</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="4"/>
-        <v>h1x9 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h1x9.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h1x9 python3 -u registryapp.py -d broker -n 8 &amp;&gt; h1x9.out &amp;</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -790,7 +790,7 @@
       </c>
       <c r="B12" t="str">
         <f>IF(COUNTIF($B$2:$B11,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B11,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B11,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B11,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>registryapp.py</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -805,8 +805,8 @@
         <v>h1x10</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="4"/>
-        <v>h1x10 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h1x10.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h1x10 python3 -u registryapp.py -d broker -n 9 &amp;&gt; h1x10.out &amp;</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -816,7 +816,7 @@
       </c>
       <c r="B13" t="str">
         <f>IF(COUNTIF($B$2:$B12,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B12,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B12,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B12,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>brokerapp.py</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -831,8 +831,8 @@
         <v>h2x1</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="4"/>
-        <v>h2x1 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x1.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h2x1 python3 -u brokerapp.py -r 10.0.0.2 -n 10 &amp;&gt; h2x1.out &amp;</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -857,7 +857,7 @@
         <v>h2x2</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h2x2 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x2.out &amp;</v>
       </c>
     </row>
@@ -883,7 +883,7 @@
         <v>h2x3</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h2x3 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x3.out &amp;</v>
       </c>
     </row>
@@ -909,7 +909,7 @@
         <v>h2x4</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h2x4 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x4.out &amp;</v>
       </c>
     </row>
@@ -935,7 +935,7 @@
         <v>h2x5</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h2x5 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x5.out &amp;</v>
       </c>
     </row>
@@ -961,7 +961,7 @@
         <v>h2x6</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h2x6 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x6.out &amp;</v>
       </c>
     </row>
@@ -987,7 +987,7 @@
         <v>h2x7</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h2x7 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x7.out &amp;</v>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
         <v>h2x8</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h2x8 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x8.out &amp;</v>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
         <v>h2x9</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h2x9 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x9.out &amp;</v>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
         <v>h2x10</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h2x10 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h2x10.out &amp;</v>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
         <v>h3x1</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x1 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x1.out &amp;</v>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
         <v>h3x2</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x2 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x2.out &amp;</v>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
         <v>h3x3</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x3 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x3.out &amp;</v>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
         <v>h3x4</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x4 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x4.out &amp;</v>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
         <v>h3x5</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x5 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x5.out &amp;</v>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
         <v>h3x6</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x6 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x6.out &amp;</v>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
         <v>h3x7</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x7 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x7.out &amp;</v>
       </c>
     </row>
@@ -1273,7 +1273,7 @@
         <v>h3x8</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x8 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x8.out &amp;</v>
       </c>
     </row>
@@ -1299,7 +1299,7 @@
         <v>h3x9</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x9 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x9.out &amp;</v>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
         <v>h3x10</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h3x10 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h3x10.out &amp;</v>
       </c>
     </row>
@@ -1351,7 +1351,7 @@
         <v>h4x1</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x1 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x1.out &amp;</v>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
         <v>h4x2</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x2 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x2.out &amp;</v>
       </c>
     </row>
@@ -1403,7 +1403,7 @@
         <v>h4x3</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x3 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x3.out &amp;</v>
       </c>
     </row>
@@ -1429,7 +1429,7 @@
         <v>h4x4</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x4 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x4.out &amp;</v>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
         <v>h4x5</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x5 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x5.out &amp;</v>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
         <v>h4x6</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x6 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x6.out &amp;</v>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
         <v>h4x7</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x7 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x7.out &amp;</v>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
         <v>h4x8</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x8 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x8.out &amp;</v>
       </c>
     </row>
@@ -1559,7 +1559,7 @@
         <v>h4x9</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x9 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x9.out &amp;</v>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
         <v>h4x10</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h4x10 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h4x10.out &amp;</v>
       </c>
     </row>
@@ -1611,7 +1611,7 @@
         <v>h5x1</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x1 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x1.out &amp;</v>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
         <v>h5x2</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x2 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x2.out &amp;</v>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
         <v>h5x3</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x3 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x3.out &amp;</v>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
         <v>h5x4</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x4 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x4.out &amp;</v>
       </c>
     </row>
@@ -1715,7 +1715,7 @@
         <v>h5x5</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x5 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x5.out &amp;</v>
       </c>
     </row>
@@ -1741,7 +1741,7 @@
         <v>h5x6</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x6 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x6.out &amp;</v>
       </c>
     </row>
@@ -1767,7 +1767,7 @@
         <v>h5x7</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x7 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x7.out &amp;</v>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
         <v>h5x8</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x8 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x8.out &amp;</v>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
         <v>h5x9</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x9 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x9.out &amp;</v>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
         <v>h5x10</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h5x10 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h5x10.out &amp;</v>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
         <v>h6x1</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>h6x1 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x1.out &amp;</v>
       </c>
     </row>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="B54" t="str">
         <f>IF(COUNTIF($B$2:$B53,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B53,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B53,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B53,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
@@ -1897,8 +1897,8 @@
         <v>h6x2</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="4"/>
-        <v>h6x2 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h6x2.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h6x2 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x2.out &amp;</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="B55" t="str">
         <f>IF(COUNTIF($B$2:$B54,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B54,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B54,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B54,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
@@ -1923,8 +1923,8 @@
         <v>h6x3</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="4"/>
-        <v>h6x3 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h6x3.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h6x3 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x3.out &amp;</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1934,7 +1934,7 @@
       </c>
       <c r="B56" t="str">
         <f>IF(COUNTIF($B$2:$B55,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B55,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B55,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B55,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
@@ -1949,8 +1949,8 @@
         <v>h6x4</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="4"/>
-        <v>h6x4 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h6x4.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h6x4 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x4.out &amp;</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="B57" t="str">
         <f>IF(COUNTIF($B$2:$B56,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B56,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B56,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B56,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
@@ -1975,8 +1975,8 @@
         <v>h6x5</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="4"/>
-        <v>h6x5 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h6x5.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h6x5 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x5.out &amp;</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="B58" t="str">
         <f>IF(COUNTIF($B$2:$B57,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B57,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B57,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B57,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
@@ -2001,8 +2001,8 @@
         <v>h6x6</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="4"/>
-        <v>h6x6 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h6x6.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h6x6 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x6.out &amp;</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="B59" t="str">
         <f>IF(COUNTIF($B$2:$B58,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B58,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B58,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B58,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
@@ -2027,8 +2027,8 @@
         <v>h6x7</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="4"/>
-        <v>h6x7 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h6x7.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h6x7 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x7.out &amp;</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="B60" t="str">
         <f>IF(COUNTIF($B$2:$B59,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B59,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B59,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B59,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
@@ -2053,8 +2053,8 @@
         <v>h6x8</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="4"/>
-        <v>h6x8 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h6x8.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h6x8 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x8.out &amp;</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2064,7 +2064,7 @@
       </c>
       <c r="B61" t="str">
         <f>IF(COUNTIF($B$2:$B60,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B60,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B60,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B60,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
@@ -2079,8 +2079,8 @@
         <v>h6x9</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="4"/>
-        <v>h6x9 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h6x9.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h6x9 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x9.out &amp;</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="B62" t="str">
         <f>IF(COUNTIF($B$2:$B61,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B61,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B61,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B61,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
@@ -2105,8 +2105,8 @@
         <v>h6x10</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="4"/>
-        <v>h6x10 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h6x10.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h6x10 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h6x10.out &amp;</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="B63" t="str">
         <f>IF(COUNTIF($B$2:$B62,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B62,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B62,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B62,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
@@ -2131,8 +2131,8 @@
         <v>h7x1</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="4"/>
-        <v>h7x1 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x1.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h7x1 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h7x1.out &amp;</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2157,8 +2157,8 @@
         <v>h7x2</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="4"/>
-        <v>h7x2 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x2.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h7x2 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h7x2.out &amp;</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2183,8 +2183,8 @@
         <v>h7x3</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="4"/>
-        <v>h7x3 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x3.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h7x3 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h7x3.out &amp;</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2209,8 +2209,8 @@
         <v>h7x4</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="4"/>
-        <v>h7x4 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x4.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h7x4 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h7x4.out &amp;</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2235,8 +2235,8 @@
         <v>h7x5</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="4"/>
-        <v>h7x5 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x5.out &amp;</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>h7x5 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h7x5.out &amp;</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2261,8 +2261,8 @@
         <v>h7x6</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" ref="F68:F105" si="9">IF($A68="","",_xlfn.CONCAT(E68," python3 -u ",$B68,IF(AND($A68=1,$B$1&gt;0)," -d broker",""),IF($B68=$G$1,_xlfn.CONCAT(" -c ",$D$1," -s ",$F$1),"")," -r 10.0.0.1 &amp;&gt; ",$E68,".out &amp;"))</f>
-        <v>h7x6 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x6.out &amp;</v>
+        <f t="shared" ref="F68:F105" ca="1" si="9">IF($A68="","",_xlfn.CONCAT(E68," python3 -u ",$B68,IF(AND(B68=$G$1,$B$1&gt;0)," -d broker",""),IF(B68=$G$1,IF(A68=1,"",_xlfn.CONCAT(" -n ",A68-1)),_xlfn.CONCAT(" -r 10.0.0.",IF(OR(B68=$A$1,B68=$E$1),RANDBETWEEN(1,$H$1),1))),IF(OR(B68=$A$1,B68=$E$1),_xlfn.CONCAT(" -n ",$H$1),"")," &amp;&gt; ",$E68,".out &amp;"))</f>
+        <v>h7x6 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h7x6.out &amp;</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2287,8 +2287,8 @@
         <v>h7x7</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="9"/>
-        <v>h7x7 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x7.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h7x7 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h7x7.out &amp;</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2313,8 +2313,8 @@
         <v>h7x8</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="9"/>
-        <v>h7x8 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x8.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h7x8 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h7x8.out &amp;</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2339,8 +2339,8 @@
         <v>h7x9</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="9"/>
-        <v>h7x9 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x9.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h7x9 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h7x9.out &amp;</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2365,8 +2365,8 @@
         <v>h7x10</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="9"/>
-        <v>h7x10 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h7x10.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h7x10 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h7x10.out &amp;</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2391,8 +2391,8 @@
         <v>h8x1</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x1 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x1.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x1 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h8x1.out &amp;</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2417,8 +2417,8 @@
         <v>h8x2</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x2 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x2.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x2 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h8x2.out &amp;</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2443,8 +2443,8 @@
         <v>h8x3</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x3 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x3.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x3 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h8x3.out &amp;</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2469,8 +2469,8 @@
         <v>h8x4</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x4 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x4.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x4 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h8x4.out &amp;</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2495,8 +2495,8 @@
         <v>h8x5</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x5 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x5.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x5 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h8x5.out &amp;</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2521,8 +2521,8 @@
         <v>h8x6</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x6 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x6.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x6 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h8x6.out &amp;</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2547,8 +2547,8 @@
         <v>h8x7</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x7 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x7.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x7 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h8x7.out &amp;</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2573,8 +2573,8 @@
         <v>h8x8</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x8 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x8.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x8 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h8x8.out &amp;</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2599,8 +2599,8 @@
         <v>h8x9</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x9 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x9.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x9 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h8x9.out &amp;</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2625,8 +2625,8 @@
         <v>h8x10</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="9"/>
-        <v>h8x10 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h8x10.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h8x10 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h8x10.out &amp;</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2651,8 +2651,8 @@
         <v>h9x1</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x1 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x1.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x1 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h9x1.out &amp;</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2677,8 +2677,8 @@
         <v>h9x2</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x2 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x2.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x2 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h9x2.out &amp;</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2703,8 +2703,8 @@
         <v>h9x3</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x3 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x3.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x3 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h9x3.out &amp;</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2729,8 +2729,8 @@
         <v>h9x4</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x4 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x4.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x4 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h9x4.out &amp;</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2755,8 +2755,8 @@
         <v>h9x5</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x5 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x5.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x5 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h9x5.out &amp;</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -2781,8 +2781,8 @@
         <v>h9x6</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x6 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x6.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x6 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h9x6.out &amp;</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -2807,8 +2807,8 @@
         <v>h9x7</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x7 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x7.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x7 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h9x7.out &amp;</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2833,8 +2833,8 @@
         <v>h9x8</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x8 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x8.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x8 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h9x8.out &amp;</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -2859,8 +2859,8 @@
         <v>h9x9</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x9 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x9.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x9 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h9x9.out &amp;</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -2885,8 +2885,8 @@
         <v>h9x10</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="9"/>
-        <v>h9x10 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h9x10.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h9x10 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h9x10.out &amp;</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -2911,8 +2911,8 @@
         <v>h10x1</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x1 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x1.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x1 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h10x1.out &amp;</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2937,8 +2937,8 @@
         <v>h10x2</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x2 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x2.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x2 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h10x2.out &amp;</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -2963,8 +2963,8 @@
         <v>h10x3</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x3 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x3.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x3 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h10x3.out &amp;</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -2989,8 +2989,8 @@
         <v>h10x4</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x4 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x4.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x4 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h10x4.out &amp;</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -3015,8 +3015,8 @@
         <v>h10x5</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x5 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x5.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x5 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h10x5.out &amp;</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -3041,8 +3041,8 @@
         <v>h10x6</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x6 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x6.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x6 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h10x6.out &amp;</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -3067,8 +3067,8 @@
         <v>h10x7</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x7 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x7.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x7 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h10x7.out &amp;</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -3093,8 +3093,8 @@
         <v>h10x8</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x8 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x8.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x8 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h10x8.out &amp;</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -3119,8 +3119,8 @@
         <v>h10x9</v>
       </c>
       <c r="F101" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x9 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x9.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x9 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h10x9.out &amp;</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -3145,86 +3145,86 @@
         <v>h10x10</v>
       </c>
       <c r="F102" t="str">
-        <f t="shared" si="9"/>
-        <v>h10x10 python3 -u subapp.py -r 10.0.0.1 &amp;&gt; h10x10.out &amp;</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>h10x10 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h10x10.out &amp;</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="A103">
+        <f t="shared" si="8"/>
+        <v>101</v>
       </c>
       <c r="B103" t="str">
         <f>IF(COUNTIF($B$2:$B102,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B102,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B102,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B102,$E$1)&lt;$F$1,$E$1,""))))</f>
+        <v>subapp.py</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="C103" t="str">
-        <f t="shared" si="5"/>
+      <c r="D103" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="D103" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
       <c r="E103" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>h101</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+        <f t="shared" ca="1" si="9"/>
+        <v>h101 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h101.out &amp;</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="A104">
+        <f t="shared" si="8"/>
+        <v>102</v>
       </c>
       <c r="B104" t="str">
         <f>IF(COUNTIF($B$2:$B103,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B103,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B103,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B103,$E$1)&lt;$F$1,$E$1,""))))</f>
+        <v>subapp.py</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="C104" t="str">
-        <f t="shared" si="5"/>
+      <c r="D104" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="D104" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
       <c r="E104" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>h102</v>
       </c>
       <c r="F104" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+        <f t="shared" ca="1" si="9"/>
+        <v>h102 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h102.out &amp;</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="A105">
+        <f t="shared" si="8"/>
+        <v>103</v>
       </c>
       <c r="B105" t="str">
         <f>IF(COUNTIF($B$2:$B104,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B104,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B104,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B104,$E$1)&lt;$F$1,$E$1,""))))</f>
+        <v>subapp.py</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="C105" t="str">
-        <f t="shared" si="5"/>
+      <c r="D105" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="D105" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
       <c r="E105" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>h103</v>
       </c>
       <c r="F105" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+        <f t="shared" ca="1" si="9"/>
+        <v>h103 python3 -u subapp.py -r 10.0.0.1 -n 10 &amp;&gt; h103.out &amp;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update testgen and setup simple tests
</commit_message>
<xml_diff>
--- a/tests/sourcegen.xlsx
+++ b/tests/sourcegen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenrees/PycharmProjects/CS6381/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDF4B98-2294-F24A-A60A-E3FD53592848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74592224-14E2-3F47-93B7-E0BCDE3C1518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2500" windowWidth="27240" windowHeight="16440" xr2:uid="{3BD69431-E4D0-FC4E-B40B-EBF74BC55B51}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>brokerapp.py</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Hostname</t>
+  </si>
+  <si>
+    <t>zookeeper</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD828EF6-56DA-5E40-88C5-762B8AEF9ABE}">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:M141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,7 +497,7 @@
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -511,13 +514,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="2">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>4</v>
@@ -528,8 +531,14 @@
       <c r="K1" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -549,14 +558,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>IF(OR(A2=$B$1+$D$1+$F$1+$H$1,A2=""),"",A2+1)</f>
+        <f>IF(OR(A2=$B$1+$D$1+$F$1+$H$1+1,A2=""),"",A2+1)</f>
         <v>1</v>
       </c>
       <c r="B3" t="str">
-        <f>IF(COUNTIF($B$2:$B2,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B2,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B2,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B2,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>registryapp.py</v>
+        <f>IF(A3=1,"zookeeper",IF(COUNTIF($B$2:$B2,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B2,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B2,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B2,$E$1)&lt;$F$1,$E$1,"")))))</f>
+        <v>zookeeper</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C66" si="0">IF(AND($A2&lt;$J$1*$K$1,ISNUMBER($A3)),CEILING($A3/$K$1,1),"")</f>
@@ -571,13 +580,13 @@
         <v>h1</v>
       </c>
       <c r="F3" t="str">
-        <f ca="1">IF($A3="","",_xlfn.CONCAT(E3," python3 -u ",$B3,IF(AND(B3=$G$1,$B$1&gt;0)," -d broker",""),IF(B3=$G$1,IF(A3=1,"",_xlfn.CONCAT(" -n ",A3-1)),_xlfn.CONCAT(" -r 10.0.0.",IF(OR(B3=$A$1,B3=$E$1),RANDBETWEEN(1,$H$1),1))),IF(OR(B3=$A$1,B3=$E$1),_xlfn.CONCAT(" -n ",$H$1),"")," &amp;&gt; ",$E3,".out &amp;"))</f>
-        <v>h1 python3 -u registryapp.py &amp;&gt; h1.out &amp;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <f>IF(A3="","",IF(B3=$L$1,"h1 ../apache-zookeeper-3.7.0-bin/bin/zkServer.sh&amp; &amp;&amp; zooinspector&amp;",_xlfn.CONCAT(E3," python3 -u ",B3,IF(AND(B3=$G$1,$B$1&gt;0)," -d broker","")," &amp;&gt; ",E3,".out &amp;")))</f>
+        <v>h1 ../apache-zookeeper-3.7.0-bin/bin/zkServer.sh&amp; &amp;&amp; zooinspector&amp;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f t="shared" ref="A4:A67" si="3">IF(OR(A3=$B$1+$D$1+$F$1+$H$1,A3=""),"",A3+1)</f>
+        <f t="shared" ref="A4:A67" si="3">IF(OR(A3=$B$1+$D$1+$F$1+$H$1+1,A3=""),"",A3+1)</f>
         <v>2</v>
       </c>
       <c r="B4" t="str">
@@ -597,11 +606,11 @@
         <v>h2</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F67" ca="1" si="4">IF($A4="","",_xlfn.CONCAT(E4," python3 -u ",$B4,IF(AND(B4=$G$1,$B$1&gt;0)," -d broker",""),IF(B4=$G$1,IF(A4=1,"",_xlfn.CONCAT(" -n ",A4-1)),_xlfn.CONCAT(" -r 10.0.0.",IF(OR(B4=$A$1,B4=$E$1),RANDBETWEEN(1,$H$1),1))),IF(OR(B4=$A$1,B4=$E$1),_xlfn.CONCAT(" -n ",$H$1),"")," &amp;&gt; ",$E4,".out &amp;"))</f>
-        <v>h2 python3 -u registryapp.py -n 1 &amp;&gt; h2.out &amp;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F4:F67" si="4">IF(A4="","",IF(B4=$L$1,"h1 ../apache-zookeeper-3.7.0-bin/bin/zkServer.sh&amp; &amp;&amp; zooinspector&amp;",_xlfn.CONCAT(E4," python3 -u ",B4,IF(AND(B4=$G$1,$B$1&gt;0)," -d broker","")," &amp;&gt; ",E4,".out &amp;")))</f>
+        <v>h2 python3 -u registryapp.py &amp;&gt; h2.out &amp;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -623,11 +632,11 @@
         <v>h3</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h3 python3 -u registryapp.py -n 2 &amp;&gt; h3.out &amp;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h3 python3 -u registryapp.py &amp;&gt; h3.out &amp;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -649,11 +658,11 @@
         <v>h4</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h4 python3 -u registryapp.py -n 3 &amp;&gt; h4.out &amp;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h4 python3 -u registryapp.py &amp;&gt; h4.out &amp;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -675,11 +684,11 @@
         <v>h5</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h5 python3 -u registryapp.py -n 4 &amp;&gt; h5.out &amp;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h5 python3 -u registryapp.py &amp;&gt; h5.out &amp;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -701,18 +710,18 @@
         <v>h6</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h6 python3 -u registryapp.py -n 5 &amp;&gt; h6.out &amp;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h6 python3 -u registryapp.py &amp;&gt; h6.out &amp;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B9" t="str">
         <f>IF(COUNTIF($B$2:$B8,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B8,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B8,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B8,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>registryapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -727,18 +736,18 @@
         <v>h7</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h7 python3 -u registryapp.py -n 6 &amp;&gt; h7.out &amp;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h7 python3 -u pubapp.py &amp;&gt; h7.out &amp;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B10" t="str">
         <f>IF(COUNTIF($B$2:$B9,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B9,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B9,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B9,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>registryapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -753,18 +762,18 @@
         <v>h8</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h8 python3 -u registryapp.py -n 7 &amp;&gt; h8.out &amp;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h8 python3 -u pubapp.py &amp;&gt; h8.out &amp;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B11" t="str">
         <f>IF(COUNTIF($B$2:$B10,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B10,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B10,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B10,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>registryapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -779,18 +788,18 @@
         <v>h9</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h9 python3 -u registryapp.py -n 8 &amp;&gt; h9.out &amp;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h9 python3 -u pubapp.py &amp;&gt; h9.out &amp;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B12" t="str">
         <f>IF(COUNTIF($B$2:$B11,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B11,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B11,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B11,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>registryapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -805,11 +814,11 @@
         <v>h10</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h10 python3 -u registryapp.py -n 9 &amp;&gt; h10.out &amp;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h10 python3 -u pubapp.py &amp;&gt; h10.out &amp;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -831,11 +840,11 @@
         <v>h11</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h11 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h11.out &amp;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h11 python3 -u pubapp.py &amp;&gt; h11.out &amp;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -857,11 +866,11 @@
         <v>h12</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h12 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h12.out &amp;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h12 python3 -u pubapp.py &amp;&gt; h12.out &amp;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -883,11 +892,11 @@
         <v>h13</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h13 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h13.out &amp;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>h13 python3 -u pubapp.py &amp;&gt; h13.out &amp;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -909,8 +918,8 @@
         <v>h14</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h14 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h14.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h14 python3 -u pubapp.py &amp;&gt; h14.out &amp;</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -935,8 +944,8 @@
         <v>h15</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h15 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h15.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h15 python3 -u pubapp.py &amp;&gt; h15.out &amp;</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -961,8 +970,8 @@
         <v>h16</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h16 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h16.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h16 python3 -u pubapp.py &amp;&gt; h16.out &amp;</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -972,7 +981,7 @@
       </c>
       <c r="B19" t="str">
         <f>IF(COUNTIF($B$2:$B18,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B18,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B18,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B18,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>subapp.py</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -987,8 +996,8 @@
         <v>h17</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h17 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h17.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h17 python3 -u subapp.py &amp;&gt; h17.out &amp;</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -998,7 +1007,7 @@
       </c>
       <c r="B20" t="str">
         <f>IF(COUNTIF($B$2:$B19,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B19,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B19,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B19,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>subapp.py</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -1013,8 +1022,8 @@
         <v>h18</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h18 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h18.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h18 python3 -u subapp.py &amp;&gt; h18.out &amp;</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1024,7 +1033,7 @@
       </c>
       <c r="B21" t="str">
         <f>IF(COUNTIF($B$2:$B20,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B20,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B20,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B20,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>subapp.py</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -1039,8 +1048,8 @@
         <v>h19</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h19 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h19.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h19 python3 -u subapp.py &amp;&gt; h19.out &amp;</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1050,7 +1059,7 @@
       </c>
       <c r="B22" t="str">
         <f>IF(COUNTIF($B$2:$B21,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B21,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B21,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B21,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>subapp.py</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -1065,8 +1074,8 @@
         <v>h20</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h20 python3 -u pubapp.py -r 10.0.0.1 &amp;&gt; h20.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h20 python3 -u subapp.py &amp;&gt; h20.out &amp;</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1091,8 +1100,8 @@
         <v>h21</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h21 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h21.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h21 python3 -u subapp.py &amp;&gt; h21.out &amp;</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1117,8 +1126,8 @@
         <v>h22</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h22 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h22.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h22 python3 -u subapp.py &amp;&gt; h22.out &amp;</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1143,8 +1152,8 @@
         <v>h23</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h23 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h23.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h23 python3 -u subapp.py &amp;&gt; h23.out &amp;</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1169,8 +1178,8 @@
         <v>h24</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h24 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h24.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h24 python3 -u subapp.py &amp;&gt; h24.out &amp;</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1195,8 +1204,8 @@
         <v>h25</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h25 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h25.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h25 python3 -u subapp.py &amp;&gt; h25.out &amp;</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1221,18 +1230,18 @@
         <v>h26</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h26 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h26.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v>h26 python3 -u subapp.py &amp;&gt; h26.out &amp;</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <f t="shared" si="3"/>
-        <v>27</v>
+      <c r="A29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B29" t="str">
         <f>IF(COUNTIF($B$2:$B28,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B28,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B28,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B28,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -1244,21 +1253,21 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="2"/>
-        <v>h27</v>
+        <v/>
       </c>
       <c r="F29" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h27 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h27.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <f t="shared" si="3"/>
-        <v>28</v>
+      <c r="A30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B30" t="str">
         <f>IF(COUNTIF($B$2:$B29,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B29,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B29,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B29,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1270,21 +1279,21 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="2"/>
-        <v>h28</v>
+        <v/>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h28 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h28.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <f t="shared" si="3"/>
-        <v>29</v>
+      <c r="A31" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B31" t="str">
         <f>IF(COUNTIF($B$2:$B30,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B30,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B30,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B30,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -1296,21 +1305,21 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="2"/>
-        <v>h29</v>
+        <v/>
       </c>
       <c r="F31" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h29 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h29.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <f t="shared" si="3"/>
-        <v>30</v>
+      <c r="A32" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B32" t="str">
         <f>IF(COUNTIF($B$2:$B31,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B31,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B31,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B31,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1322,21 +1331,21 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="2"/>
-        <v>h30</v>
+        <v/>
       </c>
       <c r="F32" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h30 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h30.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <f t="shared" si="3"/>
-        <v>31</v>
+      <c r="A33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B33" t="str">
         <f>IF(COUNTIF($B$2:$B32,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B32,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B32,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B32,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -1348,21 +1357,21 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="2"/>
-        <v>h31</v>
+        <v/>
       </c>
       <c r="F33" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h31 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h31.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <f t="shared" si="3"/>
-        <v>32</v>
+      <c r="A34" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B34" t="str">
         <f>IF(COUNTIF($B$2:$B33,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B33,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B33,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B33,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1374,21 +1383,21 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="2"/>
-        <v>h32</v>
+        <v/>
       </c>
       <c r="F34" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h32 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h32.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <f t="shared" si="3"/>
-        <v>33</v>
+      <c r="A35" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B35" t="str">
         <f>IF(COUNTIF($B$2:$B34,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B34,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B34,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B34,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -1400,21 +1409,21 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="2"/>
-        <v>h33</v>
+        <v/>
       </c>
       <c r="F35" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h33 python3 -u subapp.py -r 10.0.0.1 -n 10 &amp;&gt; h33.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <f t="shared" si="3"/>
-        <v>34</v>
+      <c r="A36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B36" t="str">
         <f>IF(COUNTIF($B$2:$B35,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B35,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B35,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B35,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -1426,21 +1435,21 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="2"/>
-        <v>h34</v>
+        <v/>
       </c>
       <c r="F36" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h34 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h34.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <f t="shared" si="3"/>
-        <v>35</v>
+      <c r="A37" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B37" t="str">
         <f>IF(COUNTIF($B$2:$B36,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B36,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B36,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B36,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -1452,21 +1461,21 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="2"/>
-        <v>h35</v>
+        <v/>
       </c>
       <c r="F37" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h35 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h35.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <f t="shared" si="3"/>
-        <v>36</v>
+      <c r="A38" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B38" t="str">
         <f>IF(COUNTIF($B$2:$B37,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B37,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B37,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B37,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -1478,21 +1487,21 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="2"/>
-        <v>h36</v>
+        <v/>
       </c>
       <c r="F38" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h36 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h36.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <f t="shared" si="3"/>
-        <v>37</v>
+      <c r="A39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B39" t="str">
         <f>IF(COUNTIF($B$2:$B38,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B38,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B38,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B38,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
@@ -1504,21 +1513,21 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="2"/>
-        <v>h37</v>
+        <v/>
       </c>
       <c r="F39" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h37 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h37.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <f t="shared" si="3"/>
-        <v>38</v>
+      <c r="A40" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B40" t="str">
         <f>IF(COUNTIF($B$2:$B39,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B39,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B39,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B39,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -1530,21 +1539,21 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="2"/>
-        <v>h38</v>
+        <v/>
       </c>
       <c r="F40" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h38 python3 -u subapp.py -r 10.0.0.1 -n 10 &amp;&gt; h38.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <f t="shared" si="3"/>
-        <v>39</v>
+      <c r="A41" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B41" t="str">
         <f>IF(COUNTIF($B$2:$B40,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B40,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B40,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B40,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
@@ -1556,21 +1565,21 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="2"/>
-        <v>h39</v>
+        <v/>
       </c>
       <c r="F41" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h39 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h39.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <f t="shared" si="3"/>
-        <v>40</v>
+      <c r="A42" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B42" t="str">
         <f>IF(COUNTIF($B$2:$B41,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B41,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B41,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B41,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
@@ -1582,21 +1591,21 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="2"/>
-        <v>h40</v>
+        <v/>
       </c>
       <c r="F42" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h40 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h40.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <f t="shared" si="3"/>
-        <v>41</v>
+      <c r="A43" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B43" t="str">
         <f>IF(COUNTIF($B$2:$B42,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B42,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B42,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B42,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
@@ -1608,21 +1617,21 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="2"/>
-        <v>h41</v>
+        <v/>
       </c>
       <c r="F43" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h41 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h41.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <f t="shared" si="3"/>
-        <v>42</v>
+      <c r="A44" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B44" t="str">
         <f>IF(COUNTIF($B$2:$B43,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B43,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B43,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B43,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
@@ -1634,21 +1643,21 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="2"/>
-        <v>h42</v>
+        <v/>
       </c>
       <c r="F44" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h42 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h42.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <f t="shared" si="3"/>
-        <v>43</v>
+      <c r="A45" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B45" t="str">
         <f>IF(COUNTIF($B$2:$B44,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B44,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B44,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B44,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
@@ -1660,21 +1669,21 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="2"/>
-        <v>h43</v>
+        <v/>
       </c>
       <c r="F45" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h43 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h43.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <f t="shared" si="3"/>
-        <v>44</v>
+      <c r="A46" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B46" t="str">
         <f>IF(COUNTIF($B$2:$B45,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B45,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B45,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B45,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
@@ -1686,21 +1695,21 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="2"/>
-        <v>h44</v>
+        <v/>
       </c>
       <c r="F46" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h44 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h44.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <f t="shared" si="3"/>
-        <v>45</v>
+      <c r="A47" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B47" t="str">
         <f>IF(COUNTIF($B$2:$B46,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B46,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B46,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B46,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
@@ -1712,21 +1721,21 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="2"/>
-        <v>h45</v>
+        <v/>
       </c>
       <c r="F47" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h45 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h45.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <f t="shared" si="3"/>
-        <v>46</v>
+      <c r="A48" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B48" t="str">
         <f>IF(COUNTIF($B$2:$B47,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B47,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B47,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B47,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
@@ -1738,21 +1747,21 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="2"/>
-        <v>h46</v>
+        <v/>
       </c>
       <c r="F48" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h46 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h46.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <f t="shared" si="3"/>
-        <v>47</v>
+      <c r="A49" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B49" t="str">
         <f>IF(COUNTIF($B$2:$B48,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B48,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B48,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B48,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
@@ -1764,21 +1773,21 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="2"/>
-        <v>h47</v>
+        <v/>
       </c>
       <c r="F49" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h47 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h47.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <f t="shared" si="3"/>
-        <v>48</v>
+      <c r="A50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B50" t="str">
         <f>IF(COUNTIF($B$2:$B49,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B49,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B49,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B49,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
@@ -1790,21 +1799,21 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="2"/>
-        <v>h48</v>
+        <v/>
       </c>
       <c r="F50" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h48 python3 -u subapp.py -r 10.0.0.1 -n 10 &amp;&gt; h48.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <f t="shared" si="3"/>
-        <v>49</v>
+      <c r="A51" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B51" t="str">
         <f>IF(COUNTIF($B$2:$B50,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B50,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B50,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B50,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
@@ -1816,21 +1825,21 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="2"/>
-        <v>h49</v>
+        <v/>
       </c>
       <c r="F51" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h49 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h49.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <f t="shared" si="3"/>
-        <v>50</v>
+      <c r="A52" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B52" t="str">
         <f>IF(COUNTIF($B$2:$B51,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B51,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B51,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B51,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
@@ -1842,21 +1851,21 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="2"/>
-        <v>h50</v>
+        <v/>
       </c>
       <c r="F52" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h50 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h50.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <f t="shared" si="3"/>
-        <v>51</v>
+      <c r="A53" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B53" t="str">
         <f>IF(COUNTIF($B$2:$B52,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B52,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B52,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B52,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
@@ -1868,21 +1877,21 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="2"/>
-        <v>h51</v>
+        <v/>
       </c>
       <c r="F53" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h51 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h51.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <f t="shared" si="3"/>
-        <v>52</v>
+      <c r="A54" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B54" t="str">
         <f>IF(COUNTIF($B$2:$B53,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B53,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B53,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B53,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
@@ -1894,21 +1903,21 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="2"/>
-        <v>h52</v>
+        <v/>
       </c>
       <c r="F54" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h52 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h52.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <f t="shared" si="3"/>
-        <v>53</v>
+      <c r="A55" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B55" t="str">
         <f>IF(COUNTIF($B$2:$B54,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B54,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B54,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B54,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
@@ -1920,21 +1929,21 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="2"/>
-        <v>h53</v>
+        <v/>
       </c>
       <c r="F55" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h53 python3 -u subapp.py -r 10.0.0.1 -n 10 &amp;&gt; h53.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <f t="shared" si="3"/>
-        <v>54</v>
+      <c r="A56" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B56" t="str">
         <f>IF(COUNTIF($B$2:$B55,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B55,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B55,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B55,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
@@ -1946,21 +1955,21 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="2"/>
-        <v>h54</v>
+        <v/>
       </c>
       <c r="F56" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h54 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h54.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <f t="shared" si="3"/>
-        <v>55</v>
+      <c r="A57" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B57" t="str">
         <f>IF(COUNTIF($B$2:$B56,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B56,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B56,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B56,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
@@ -1972,21 +1981,21 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="2"/>
-        <v>h55</v>
+        <v/>
       </c>
       <c r="F57" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h55 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h55.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <f t="shared" si="3"/>
-        <v>56</v>
+      <c r="A58" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B58" t="str">
         <f>IF(COUNTIF($B$2:$B57,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B57,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B57,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B57,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
@@ -1998,21 +2007,21 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="2"/>
-        <v>h56</v>
+        <v/>
       </c>
       <c r="F58" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h56 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h56.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <f t="shared" si="3"/>
-        <v>57</v>
+      <c r="A59" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B59" t="str">
         <f>IF(COUNTIF($B$2:$B58,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B58,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B58,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B58,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
@@ -2024,21 +2033,21 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="2"/>
-        <v>h57</v>
+        <v/>
       </c>
       <c r="F59" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h57 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h57.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <f t="shared" si="3"/>
-        <v>58</v>
+      <c r="A60" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B60" t="str">
         <f>IF(COUNTIF($B$2:$B59,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B59,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B59,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B59,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
@@ -2050,21 +2059,21 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="2"/>
-        <v>h58</v>
+        <v/>
       </c>
       <c r="F60" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h58 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h58.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <f t="shared" si="3"/>
-        <v>59</v>
+      <c r="A61" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B61" t="str">
         <f>IF(COUNTIF($B$2:$B60,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B60,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B60,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B60,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
@@ -2076,21 +2085,21 @@
       </c>
       <c r="E61" t="str">
         <f t="shared" si="2"/>
-        <v>h59</v>
+        <v/>
       </c>
       <c r="F61" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h59 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h59.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <f t="shared" si="3"/>
-        <v>60</v>
+      <c r="A62" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B62" t="str">
         <f>IF(COUNTIF($B$2:$B61,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B61,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B61,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B61,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
@@ -2102,21 +2111,21 @@
       </c>
       <c r="E62" t="str">
         <f t="shared" si="2"/>
-        <v>h60</v>
+        <v/>
       </c>
       <c r="F62" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h60 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h60.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <f t="shared" si="3"/>
-        <v>61</v>
+      <c r="A63" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B63" t="str">
         <f>IF(COUNTIF($B$2:$B62,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B62,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B62,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B62,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
@@ -2128,21 +2137,21 @@
       </c>
       <c r="E63" t="str">
         <f t="shared" si="2"/>
-        <v>h61</v>
+        <v/>
       </c>
       <c r="F63" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h61 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h61.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <f t="shared" si="3"/>
-        <v>62</v>
+      <c r="A64" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B64" t="str">
         <f>IF(COUNTIF($B$2:$B63,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B63,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B63,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B63,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
@@ -2154,21 +2163,21 @@
       </c>
       <c r="E64" t="str">
         <f t="shared" si="2"/>
-        <v>h62</v>
+        <v/>
       </c>
       <c r="F64" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h62 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h62.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <f t="shared" si="3"/>
-        <v>63</v>
+      <c r="A65" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B65" t="str">
         <f>IF(COUNTIF($B$2:$B64,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B64,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B64,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B64,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
@@ -2180,21 +2189,21 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="2"/>
-        <v>h63</v>
+        <v/>
       </c>
       <c r="F65" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h63 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h63.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <f t="shared" si="3"/>
-        <v>64</v>
+      <c r="A66" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B66" t="str">
         <f>IF(COUNTIF($B$2:$B65,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B65,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B65,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B65,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
@@ -2206,21 +2215,21 @@
       </c>
       <c r="E66" t="str">
         <f t="shared" si="2"/>
-        <v>h64</v>
+        <v/>
       </c>
       <c r="F66" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h64 python3 -u subapp.py -r 10.0.0.1 -n 10 &amp;&gt; h64.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <f t="shared" si="3"/>
-        <v>65</v>
+      <c r="A67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="B67" t="str">
         <f>IF(COUNTIF($B$2:$B66,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B66,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B66,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B66,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C115" si="5">IF(AND($A66&lt;$J$1*$K$1,ISNUMBER($A67)),CEILING($A67/$K$1,1),"")</f>
@@ -2232,21 +2241,21 @@
       </c>
       <c r="E67" t="str">
         <f t="shared" ref="E67:E105" si="7">IF(AND(ISNUMBER(C67),ISNUMBER(D67)),_xlfn.CONCAT("h",C67,"x",D67),IF(ISNUMBER($A67),_xlfn.CONCAT("h",A67),""))</f>
-        <v>h65</v>
+        <v/>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>h65 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h65.out &amp;</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <f t="shared" ref="A68:A115" si="8">IF(OR(A67=$B$1+$D$1+$F$1+$H$1,A67=""),"",A67+1)</f>
-        <v>66</v>
+      <c r="A68" t="str">
+        <f t="shared" ref="A68:A131" si="8">IF(OR(A67=$B$1+$D$1+$F$1+$H$1+1,A67=""),"",A67+1)</f>
+        <v/>
       </c>
       <c r="B68" t="str">
         <f>IF(COUNTIF($B$2:$B67,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B67,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B67,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B67,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="5"/>
@@ -2258,21 +2267,21 @@
       </c>
       <c r="E68" t="str">
         <f t="shared" si="7"/>
-        <v>h66</v>
+        <v/>
       </c>
       <c r="F68" t="str">
-        <f t="shared" ref="F68:F105" ca="1" si="9">IF($A68="","",_xlfn.CONCAT(E68," python3 -u ",$B68,IF(AND(B68=$G$1,$B$1&gt;0)," -d broker",""),IF(B68=$G$1,IF(A68=1,"",_xlfn.CONCAT(" -n ",A68-1)),_xlfn.CONCAT(" -r 10.0.0.",IF(OR(B68=$A$1,B68=$E$1),RANDBETWEEN(1,$H$1),1))),IF(OR(B68=$A$1,B68=$E$1),_xlfn.CONCAT(" -n ",$H$1),"")," &amp;&gt; ",$E68,".out &amp;"))</f>
-        <v>h66 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h66.out &amp;</v>
+        <f t="shared" ref="F68:F119" si="9">IF(A68="","",IF(B68=$L$1,"h1 ../apache-zookeeper-3.7.0-bin/bin/zkServer.sh&amp; &amp;&amp; zooinspector&amp;",_xlfn.CONCAT(E68," python3 -u ",B68,IF(AND(B68=$G$1,$B$1&gt;0)," -d broker","")," &amp;&gt; ",E68,".out &amp;")))</f>
+        <v/>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <f t="shared" si="8"/>
-        <v>67</v>
+      <c r="A69" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B69" t="str">
         <f>IF(COUNTIF($B$2:$B68,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B68,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B68,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B68,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="5"/>
@@ -2284,21 +2293,21 @@
       </c>
       <c r="E69" t="str">
         <f t="shared" si="7"/>
-        <v>h67</v>
+        <v/>
       </c>
       <c r="F69" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h67 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h67.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <f t="shared" si="8"/>
-        <v>68</v>
+      <c r="A70" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B70" t="str">
         <f>IF(COUNTIF($B$2:$B69,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B69,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B69,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B69,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="5"/>
@@ -2310,21 +2319,21 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="7"/>
-        <v>h68</v>
+        <v/>
       </c>
       <c r="F70" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h68 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h68.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <f t="shared" si="8"/>
-        <v>69</v>
+      <c r="A71" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B71" t="str">
         <f>IF(COUNTIF($B$2:$B70,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B70,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B70,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B70,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="5"/>
@@ -2336,21 +2345,21 @@
       </c>
       <c r="E71" t="str">
         <f t="shared" si="7"/>
-        <v>h69</v>
+        <v/>
       </c>
       <c r="F71" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h69 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h69.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <f t="shared" si="8"/>
-        <v>70</v>
+      <c r="A72" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B72" t="str">
         <f>IF(COUNTIF($B$2:$B71,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B71,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B71,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B71,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="5"/>
@@ -2362,21 +2371,21 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="7"/>
-        <v>h70</v>
+        <v/>
       </c>
       <c r="F72" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h70 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h70.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <f t="shared" si="8"/>
-        <v>71</v>
+      <c r="A73" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B73" t="str">
         <f>IF(COUNTIF($B$2:$B72,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B72,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B72,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B72,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="5"/>
@@ -2388,21 +2397,21 @@
       </c>
       <c r="E73" t="str">
         <f t="shared" si="7"/>
-        <v>h71</v>
+        <v/>
       </c>
       <c r="F73" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h71 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h71.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <f t="shared" si="8"/>
-        <v>72</v>
+      <c r="A74" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B74" t="str">
         <f>IF(COUNTIF($B$2:$B73,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B73,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B73,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B73,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="5"/>
@@ -2414,21 +2423,21 @@
       </c>
       <c r="E74" t="str">
         <f t="shared" si="7"/>
-        <v>h72</v>
+        <v/>
       </c>
       <c r="F74" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h72 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h72.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <f t="shared" si="8"/>
-        <v>73</v>
+      <c r="A75" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B75" t="str">
         <f>IF(COUNTIF($B$2:$B74,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B74,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B74,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B74,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="5"/>
@@ -2440,21 +2449,21 @@
       </c>
       <c r="E75" t="str">
         <f t="shared" si="7"/>
-        <v>h73</v>
+        <v/>
       </c>
       <c r="F75" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h73 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h73.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <f t="shared" si="8"/>
-        <v>74</v>
+      <c r="A76" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B76" t="str">
         <f>IF(COUNTIF($B$2:$B75,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B75,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B75,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B75,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="5"/>
@@ -2466,21 +2475,21 @@
       </c>
       <c r="E76" t="str">
         <f t="shared" si="7"/>
-        <v>h74</v>
+        <v/>
       </c>
       <c r="F76" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h74 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h74.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <f t="shared" si="8"/>
-        <v>75</v>
+      <c r="A77" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B77" t="str">
         <f>IF(COUNTIF($B$2:$B76,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B76,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B76,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B76,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="5"/>
@@ -2492,21 +2501,21 @@
       </c>
       <c r="E77" t="str">
         <f t="shared" si="7"/>
-        <v>h75</v>
+        <v/>
       </c>
       <c r="F77" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h75 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h75.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <f t="shared" si="8"/>
-        <v>76</v>
+      <c r="A78" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B78" t="str">
         <f>IF(COUNTIF($B$2:$B77,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B77,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B77,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B77,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="5"/>
@@ -2518,21 +2527,21 @@
       </c>
       <c r="E78" t="str">
         <f t="shared" si="7"/>
-        <v>h76</v>
+        <v/>
       </c>
       <c r="F78" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h76 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h76.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <f t="shared" si="8"/>
-        <v>77</v>
+      <c r="A79" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B79" t="str">
         <f>IF(COUNTIF($B$2:$B78,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B78,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B78,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B78,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="5"/>
@@ -2544,21 +2553,21 @@
       </c>
       <c r="E79" t="str">
         <f t="shared" si="7"/>
-        <v>h77</v>
+        <v/>
       </c>
       <c r="F79" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h77 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h77.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <f t="shared" si="8"/>
-        <v>78</v>
+      <c r="A80" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B80" t="str">
         <f>IF(COUNTIF($B$2:$B79,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B79,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B79,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B79,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="5"/>
@@ -2570,21 +2579,21 @@
       </c>
       <c r="E80" t="str">
         <f t="shared" si="7"/>
-        <v>h78</v>
+        <v/>
       </c>
       <c r="F80" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h78 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h78.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <f t="shared" si="8"/>
-        <v>79</v>
+      <c r="A81" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B81" t="str">
         <f>IF(COUNTIF($B$2:$B80,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B80,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B80,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B80,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="5"/>
@@ -2596,21 +2605,21 @@
       </c>
       <c r="E81" t="str">
         <f t="shared" si="7"/>
-        <v>h79</v>
+        <v/>
       </c>
       <c r="F81" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h79 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h79.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <f t="shared" si="8"/>
-        <v>80</v>
+      <c r="A82" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B82" t="str">
         <f>IF(COUNTIF($B$2:$B81,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B81,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B81,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B81,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="5"/>
@@ -2622,21 +2631,21 @@
       </c>
       <c r="E82" t="str">
         <f t="shared" si="7"/>
-        <v>h80</v>
+        <v/>
       </c>
       <c r="F82" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h80 python3 -u subapp.py -r 10.0.0.1 -n 10 &amp;&gt; h80.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <f t="shared" si="8"/>
-        <v>81</v>
+      <c r="A83" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B83" t="str">
         <f>IF(COUNTIF($B$2:$B82,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B82,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B82,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B82,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="5"/>
@@ -2648,21 +2657,21 @@
       </c>
       <c r="E83" t="str">
         <f t="shared" si="7"/>
-        <v>h81</v>
+        <v/>
       </c>
       <c r="F83" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h81 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h81.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <f t="shared" si="8"/>
-        <v>82</v>
+      <c r="A84" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B84" t="str">
         <f>IF(COUNTIF($B$2:$B83,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B83,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B83,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B83,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="5"/>
@@ -2674,21 +2683,21 @@
       </c>
       <c r="E84" t="str">
         <f t="shared" si="7"/>
-        <v>h82</v>
+        <v/>
       </c>
       <c r="F84" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h82 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h82.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <f t="shared" si="8"/>
-        <v>83</v>
+      <c r="A85" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B85" t="str">
         <f>IF(COUNTIF($B$2:$B84,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B84,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B84,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B84,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="5"/>
@@ -2700,21 +2709,21 @@
       </c>
       <c r="E85" t="str">
         <f t="shared" si="7"/>
-        <v>h83</v>
+        <v/>
       </c>
       <c r="F85" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h83 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h83.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <f t="shared" si="8"/>
-        <v>84</v>
+      <c r="A86" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B86" t="str">
         <f>IF(COUNTIF($B$2:$B85,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B85,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B85,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B85,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="5"/>
@@ -2726,21 +2735,21 @@
       </c>
       <c r="E86" t="str">
         <f t="shared" si="7"/>
-        <v>h84</v>
+        <v/>
       </c>
       <c r="F86" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h84 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h84.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <f t="shared" si="8"/>
-        <v>85</v>
+      <c r="A87" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B87" t="str">
         <f>IF(COUNTIF($B$2:$B86,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B86,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B86,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B86,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="5"/>
@@ -2752,21 +2761,21 @@
       </c>
       <c r="E87" t="str">
         <f t="shared" si="7"/>
-        <v>h85</v>
+        <v/>
       </c>
       <c r="F87" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h85 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h85.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <f t="shared" si="8"/>
-        <v>86</v>
+      <c r="A88" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B88" t="str">
         <f>IF(COUNTIF($B$2:$B87,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B87,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B87,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B87,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="5"/>
@@ -2778,21 +2787,21 @@
       </c>
       <c r="E88" t="str">
         <f t="shared" si="7"/>
-        <v>h86</v>
+        <v/>
       </c>
       <c r="F88" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h86 python3 -u subapp.py -r 10.0.0.1 -n 10 &amp;&gt; h86.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <f t="shared" si="8"/>
-        <v>87</v>
+      <c r="A89" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B89" t="str">
         <f>IF(COUNTIF($B$2:$B88,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B88,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B88,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B88,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="5"/>
@@ -2804,21 +2813,21 @@
       </c>
       <c r="E89" t="str">
         <f t="shared" si="7"/>
-        <v>h87</v>
+        <v/>
       </c>
       <c r="F89" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h87 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h87.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <f t="shared" si="8"/>
-        <v>88</v>
+      <c r="A90" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B90" t="str">
         <f>IF(COUNTIF($B$2:$B89,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B89,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B89,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B89,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="5"/>
@@ -2830,21 +2839,21 @@
       </c>
       <c r="E90" t="str">
         <f t="shared" si="7"/>
-        <v>h88</v>
+        <v/>
       </c>
       <c r="F90" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h88 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h88.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <f t="shared" si="8"/>
-        <v>89</v>
+      <c r="A91" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B91" t="str">
         <f>IF(COUNTIF($B$2:$B90,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B90,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B90,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B90,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="5"/>
@@ -2856,21 +2865,21 @@
       </c>
       <c r="E91" t="str">
         <f t="shared" si="7"/>
-        <v>h89</v>
+        <v/>
       </c>
       <c r="F91" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h89 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h89.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <f t="shared" si="8"/>
-        <v>90</v>
+      <c r="A92" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B92" t="str">
         <f>IF(COUNTIF($B$2:$B91,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B91,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B91,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B91,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="5"/>
@@ -2882,21 +2891,21 @@
       </c>
       <c r="E92" t="str">
         <f t="shared" si="7"/>
-        <v>h90</v>
+        <v/>
       </c>
       <c r="F92" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h90 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h90.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <f t="shared" si="8"/>
-        <v>91</v>
+      <c r="A93" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B93" t="str">
         <f>IF(COUNTIF($B$2:$B92,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B92,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B92,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B92,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="5"/>
@@ -2908,21 +2917,21 @@
       </c>
       <c r="E93" t="str">
         <f t="shared" si="7"/>
-        <v>h91</v>
+        <v/>
       </c>
       <c r="F93" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h91 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h91.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <f t="shared" si="8"/>
-        <v>92</v>
+      <c r="A94" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B94" t="str">
         <f>IF(COUNTIF($B$2:$B93,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B93,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B93,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B93,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="5"/>
@@ -2934,21 +2943,21 @@
       </c>
       <c r="E94" t="str">
         <f t="shared" si="7"/>
-        <v>h92</v>
+        <v/>
       </c>
       <c r="F94" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h92 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h92.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <f t="shared" si="8"/>
-        <v>93</v>
+      <c r="A95" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B95" t="str">
         <f>IF(COUNTIF($B$2:$B94,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B94,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B94,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B94,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="5"/>
@@ -2960,21 +2969,21 @@
       </c>
       <c r="E95" t="str">
         <f t="shared" si="7"/>
-        <v>h93</v>
+        <v/>
       </c>
       <c r="F95" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h93 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h93.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <f t="shared" si="8"/>
-        <v>94</v>
+      <c r="A96" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B96" t="str">
         <f>IF(COUNTIF($B$2:$B95,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B95,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B95,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B95,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="5"/>
@@ -2986,21 +2995,21 @@
       </c>
       <c r="E96" t="str">
         <f t="shared" si="7"/>
-        <v>h94</v>
+        <v/>
       </c>
       <c r="F96" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h94 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h94.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <f t="shared" si="8"/>
-        <v>95</v>
+      <c r="A97" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B97" t="str">
         <f>IF(COUNTIF($B$2:$B96,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B96,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B96,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B96,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="5"/>
@@ -3012,21 +3021,21 @@
       </c>
       <c r="E97" t="str">
         <f t="shared" si="7"/>
-        <v>h95</v>
+        <v/>
       </c>
       <c r="F97" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h95 python3 -u subapp.py -r 10.0.0.7 -n 10 &amp;&gt; h95.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <f t="shared" si="8"/>
-        <v>96</v>
+      <c r="A98" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B98" t="str">
         <f>IF(COUNTIF($B$2:$B97,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B97,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B97,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B97,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="5"/>
@@ -3038,21 +3047,21 @@
       </c>
       <c r="E98" t="str">
         <f t="shared" si="7"/>
-        <v>h96</v>
+        <v/>
       </c>
       <c r="F98" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h96 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h96.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <f t="shared" si="8"/>
-        <v>97</v>
+      <c r="A99" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B99" t="str">
         <f>IF(COUNTIF($B$2:$B98,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B98,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B98,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B98,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="5"/>
@@ -3064,21 +3073,21 @@
       </c>
       <c r="E99" t="str">
         <f t="shared" si="7"/>
-        <v>h97</v>
+        <v/>
       </c>
       <c r="F99" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h97 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h97.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <f t="shared" si="8"/>
-        <v>98</v>
+      <c r="A100" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B100" t="str">
         <f>IF(COUNTIF($B$2:$B99,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B99,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B99,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B99,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="5"/>
@@ -3090,21 +3099,21 @@
       </c>
       <c r="E100" t="str">
         <f t="shared" si="7"/>
-        <v>h98</v>
+        <v/>
       </c>
       <c r="F100" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h98 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h98.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <f t="shared" si="8"/>
-        <v>99</v>
+      <c r="A101" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B101" t="str">
         <f>IF(COUNTIF($B$2:$B100,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B100,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B100,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B100,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="5"/>
@@ -3116,21 +3125,21 @@
       </c>
       <c r="E101" t="str">
         <f t="shared" si="7"/>
-        <v>h99</v>
+        <v/>
       </c>
       <c r="F101" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h99 python3 -u subapp.py -r 10.0.0.3 -n 10 &amp;&gt; h99.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <f t="shared" si="8"/>
-        <v>100</v>
+      <c r="A102" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B102" t="str">
         <f>IF(COUNTIF($B$2:$B101,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B101,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B101,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B101,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="5"/>
@@ -3142,21 +3151,21 @@
       </c>
       <c r="E102" t="str">
         <f t="shared" si="7"/>
-        <v>h100</v>
+        <v/>
       </c>
       <c r="F102" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h100 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h100.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <f t="shared" si="8"/>
-        <v>101</v>
+      <c r="A103" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B103" t="str">
         <f>IF(COUNTIF($B$2:$B102,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B102,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B102,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B102,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="5"/>
@@ -3168,21 +3177,21 @@
       </c>
       <c r="E103" t="str">
         <f t="shared" si="7"/>
-        <v>h101</v>
+        <v/>
       </c>
       <c r="F103" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h101 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h101.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104">
-        <f t="shared" si="8"/>
-        <v>102</v>
+      <c r="A104" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B104" t="str">
         <f>IF(COUNTIF($B$2:$B103,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B103,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B103,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B103,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="5"/>
@@ -3194,21 +3203,21 @@
       </c>
       <c r="E104" t="str">
         <f t="shared" si="7"/>
-        <v>h102</v>
+        <v/>
       </c>
       <c r="F104" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h102 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h102.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105">
-        <f t="shared" si="8"/>
-        <v>103</v>
+      <c r="A105" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B105" t="str">
         <f>IF(COUNTIF($B$2:$B104,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B104,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B104,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B104,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="5"/>
@@ -3220,21 +3229,21 @@
       </c>
       <c r="E105" t="str">
         <f t="shared" si="7"/>
-        <v>h103</v>
+        <v/>
       </c>
       <c r="F105" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>h103 python3 -u subapp.py -r 10.0.0.10 -n 10 &amp;&gt; h103.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106">
-        <f t="shared" si="8"/>
-        <v>104</v>
+      <c r="A106" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B106" t="str">
         <f>IF(COUNTIF($B$2:$B105,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B105,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B105,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B105,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="5"/>
@@ -3246,21 +3255,21 @@
       </c>
       <c r="E106" t="str">
         <f t="shared" ref="E106:E115" si="10">IF(AND(ISNUMBER(C106),ISNUMBER(D106)),_xlfn.CONCAT("h",C106,"x",D106),IF(ISNUMBER($A106),_xlfn.CONCAT("h",A106),""))</f>
-        <v>h104</v>
+        <v/>
       </c>
       <c r="F106" t="str">
-        <f t="shared" ref="F106:F115" ca="1" si="11">IF($A106="","",_xlfn.CONCAT(E106," python3 -u ",$B106,IF(AND(B106=$G$1,$B$1&gt;0)," -d broker",""),IF(B106=$G$1,IF(A106=1,"",_xlfn.CONCAT(" -n ",A106-1)),_xlfn.CONCAT(" -r 10.0.0.",IF(OR(B106=$A$1,B106=$E$1),RANDBETWEEN(1,$H$1),1))),IF(OR(B106=$A$1,B106=$E$1),_xlfn.CONCAT(" -n ",$H$1),"")," &amp;&gt; ",$E106,".out &amp;"))</f>
-        <v>h104 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h104.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <f t="shared" si="8"/>
-        <v>105</v>
+      <c r="A107" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B107" t="str">
         <f>IF(COUNTIF($B$2:$B106,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B106,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B106,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B106,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="5"/>
@@ -3272,21 +3281,21 @@
       </c>
       <c r="E107" t="str">
         <f t="shared" si="10"/>
-        <v>h105</v>
+        <v/>
       </c>
       <c r="F107" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>h105 python3 -u subapp.py -r 10.0.0.9 -n 10 &amp;&gt; h105.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <f t="shared" si="8"/>
-        <v>106</v>
+      <c r="A108" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B108" t="str">
         <f>IF(COUNTIF($B$2:$B107,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B107,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B107,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B107,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="5"/>
@@ -3298,21 +3307,21 @@
       </c>
       <c r="E108" t="str">
         <f t="shared" si="10"/>
-        <v>h106</v>
+        <v/>
       </c>
       <c r="F108" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>h106 python3 -u subapp.py -r 10.0.0.8 -n 10 &amp;&gt; h106.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109">
-        <f t="shared" si="8"/>
-        <v>107</v>
+      <c r="A109" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B109" t="str">
         <f>IF(COUNTIF($B$2:$B108,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B108,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B108,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B108,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="5"/>
@@ -3324,21 +3333,21 @@
       </c>
       <c r="E109" t="str">
         <f t="shared" si="10"/>
-        <v>h107</v>
+        <v/>
       </c>
       <c r="F109" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>h107 python3 -u subapp.py -r 10.0.0.4 -n 10 &amp;&gt; h107.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <f t="shared" si="8"/>
-        <v>108</v>
+      <c r="A110" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B110" t="str">
         <f>IF(COUNTIF($B$2:$B109,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B109,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B109,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B109,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="5"/>
@@ -3350,21 +3359,21 @@
       </c>
       <c r="E110" t="str">
         <f t="shared" si="10"/>
-        <v>h108</v>
+        <v/>
       </c>
       <c r="F110" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>h108 python3 -u subapp.py -r 10.0.0.5 -n 10 &amp;&gt; h108.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111">
-        <f t="shared" si="8"/>
-        <v>109</v>
+      <c r="A111" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B111" t="str">
         <f>IF(COUNTIF($B$2:$B110,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B110,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B110,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B110,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="5"/>
@@ -3376,21 +3385,21 @@
       </c>
       <c r="E111" t="str">
         <f t="shared" si="10"/>
-        <v>h109</v>
+        <v/>
       </c>
       <c r="F111" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>h109 python3 -u subapp.py -r 10.0.0.6 -n 10 &amp;&gt; h109.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112">
-        <f t="shared" si="8"/>
-        <v>110</v>
+      <c r="A112" t="str">
+        <f t="shared" si="8"/>
+        <v/>
       </c>
       <c r="B112" t="str">
         <f>IF(COUNTIF($B$2:$B111,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B111,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B111,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B111,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v/>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="5"/>
@@ -3402,11 +3411,11 @@
       </c>
       <c r="E112" t="str">
         <f t="shared" si="10"/>
-        <v>h110</v>
+        <v/>
       </c>
       <c r="F112" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>h110 python3 -u subapp.py -r 10.0.0.2 -n 10 &amp;&gt; h110.out &amp;</v>
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -3431,7 +3440,7 @@
         <v/>
       </c>
       <c r="F113" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3457,7 +3466,7 @@
         <v/>
       </c>
       <c r="F114" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -3483,7 +3492,179 @@
         <v/>
       </c>
       <c r="F115" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="F116" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="F117" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="F118" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="F119" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="str">
+        <f t="shared" ref="A132" si="11">IF(OR(A131=$B$1+$D$1+$F$1+$H$1+1,A131=""),"",A131+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="str">
+        <f t="shared" ref="A132:A141" si="12">IF(OR(A132=$B$1+$D$1+$F$1+$H$1,A132=""),"",A132+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="str">
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Attempt at broker balancing
</commit_message>
<xml_diff>
--- a/tests/sourcegen.xlsx
+++ b/tests/sourcegen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenrees/PycharmProjects/CS6381/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E070050-1704-F545-812E-0963AB837952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C57A03-FAA9-974E-8C0F-08FFD28551D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2500" windowWidth="27240" windowHeight="16440" xr2:uid="{3BD69431-E4D0-FC4E-B40B-EBF74BC55B51}"/>
+    <workbookView xWindow="11460" yWindow="2380" windowWidth="27240" windowHeight="16440" xr2:uid="{3BD69431-E4D0-FC4E-B40B-EBF74BC55B51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,6 +85,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -159,13 +166,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +491,7 @@
   <dimension ref="A1:M141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F3" sqref="F3:F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,25 +510,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2">
-        <v>10</v>
-      </c>
-      <c r="G1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>4</v>
@@ -607,7 +615,7 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4:F29" si="4">IF(A4="","",IF(B4=$L$1,"h1 ../apache-zookeeper-3.7.0-bin/bin/zkServer.sh start &amp;&amp; zooinspector&amp;",_xlfn.CONCAT(E4," python3 -u ",B4,IF(AND(B4=$G$1,$B$1&gt;0)," -d broker","")," &amp;&gt; ",E4,".out &amp;")))</f>
-        <v>h2 python3 -u registryapp.py &amp;&gt; h2.out &amp;</v>
+        <v>h2 python3 -u registryapp.py -d broker &amp;&gt; h2.out &amp;</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -633,7 +641,7 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" si="4"/>
-        <v>h3 python3 -u registryapp.py &amp;&gt; h3.out &amp;</v>
+        <v>h3 python3 -u registryapp.py -d broker &amp;&gt; h3.out &amp;</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -659,7 +667,7 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="4"/>
-        <v>h4 python3 -u registryapp.py &amp;&gt; h4.out &amp;</v>
+        <v>h4 python3 -u registryapp.py -d broker &amp;&gt; h4.out &amp;</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -685,7 +693,7 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="4"/>
-        <v>h5 python3 -u registryapp.py &amp;&gt; h5.out &amp;</v>
+        <v>h5 python3 -u registryapp.py -d broker &amp;&gt; h5.out &amp;</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -695,7 +703,7 @@
       </c>
       <c r="B8" t="str">
         <f>IF(COUNTIF($B$2:$B7,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B7,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B7,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B7,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>registryapp.py</v>
+        <v>brokerapp.py</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -711,7 +719,7 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="4"/>
-        <v>h6 python3 -u registryapp.py &amp;&gt; h6.out &amp;</v>
+        <v>h6 python3 -u brokerapp.py &amp;&gt; h6.out &amp;</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -721,7 +729,7 @@
       </c>
       <c r="B9" t="str">
         <f>IF(COUNTIF($B$2:$B8,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B8,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B8,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B8,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>brokerapp.py</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -737,7 +745,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="4"/>
-        <v>h7 python3 -u pubapp.py &amp;&gt; h7.out &amp;</v>
+        <v>h7 python3 -u brokerapp.py &amp;&gt; h7.out &amp;</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -747,7 +755,7 @@
       </c>
       <c r="B10" t="str">
         <f>IF(COUNTIF($B$2:$B9,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B9,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B9,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B9,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>brokerapp.py</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -763,7 +771,7 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="4"/>
-        <v>h8 python3 -u pubapp.py &amp;&gt; h8.out &amp;</v>
+        <v>h8 python3 -u brokerapp.py &amp;&gt; h8.out &amp;</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -773,7 +781,7 @@
       </c>
       <c r="B11" t="str">
         <f>IF(COUNTIF($B$2:$B10,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B10,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B10,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B10,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>pubapp.py</v>
+        <v>brokerapp.py</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -789,7 +797,7 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="4"/>
-        <v>h9 python3 -u pubapp.py &amp;&gt; h9.out &amp;</v>
+        <v>h9 python3 -u brokerapp.py &amp;&gt; h9.out &amp;</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -981,7 +989,7 @@
       </c>
       <c r="B19" t="str">
         <f>IF(COUNTIF($B$2:$B18,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B18,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B18,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B18,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -997,7 +1005,7 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="4"/>
-        <v>h17 python3 -u subapp.py &amp;&gt; h17.out &amp;</v>
+        <v>h17 python3 -u pubapp.py &amp;&gt; h17.out &amp;</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1007,7 +1015,7 @@
       </c>
       <c r="B20" t="str">
         <f>IF(COUNTIF($B$2:$B19,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B19,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B19,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B19,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -1023,7 +1031,7 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="4"/>
-        <v>h18 python3 -u subapp.py &amp;&gt; h18.out &amp;</v>
+        <v>h18 python3 -u pubapp.py &amp;&gt; h18.out &amp;</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1033,7 +1041,7 @@
       </c>
       <c r="B21" t="str">
         <f>IF(COUNTIF($B$2:$B20,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B20,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B20,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B20,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -1049,7 +1057,7 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="4"/>
-        <v>h19 python3 -u subapp.py &amp;&gt; h19.out &amp;</v>
+        <v>h19 python3 -u pubapp.py &amp;&gt; h19.out &amp;</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1059,7 +1067,7 @@
       </c>
       <c r="B22" t="str">
         <f>IF(COUNTIF($B$2:$B21,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B21,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B21,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B21,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -1075,7 +1083,7 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="4"/>
-        <v>h20 python3 -u subapp.py &amp;&gt; h20.out &amp;</v>
+        <v>h20 python3 -u pubapp.py &amp;&gt; h20.out &amp;</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1085,7 +1093,7 @@
       </c>
       <c r="B23" t="str">
         <f>IF(COUNTIF($B$2:$B22,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B22,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B22,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B22,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C23" t="str">
         <f>IF(AND($A22&lt;$J$1*$K$1,ISNUMBER($A23)),CEILING($A23/$K$1,1),"")</f>
@@ -1101,7 +1109,7 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="4"/>
-        <v>h21 python3 -u subapp.py &amp;&gt; h21.out &amp;</v>
+        <v>h21 python3 -u pubapp.py &amp;&gt; h21.out &amp;</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1111,7 +1119,7 @@
       </c>
       <c r="B24" t="str">
         <f>IF(COUNTIF($B$2:$B23,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B23,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B23,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B23,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -1127,7 +1135,7 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="4"/>
-        <v>h22 python3 -u subapp.py &amp;&gt; h22.out &amp;</v>
+        <v>h22 python3 -u pubapp.py &amp;&gt; h22.out &amp;</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1137,7 +1145,7 @@
       </c>
       <c r="B25" t="str">
         <f>IF(COUNTIF($B$2:$B24,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B24,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B24,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B24,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -1153,7 +1161,7 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="4"/>
-        <v>h23 python3 -u subapp.py &amp;&gt; h23.out &amp;</v>
+        <v>h23 python3 -u pubapp.py &amp;&gt; h23.out &amp;</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1163,7 +1171,7 @@
       </c>
       <c r="B26" t="str">
         <f>IF(COUNTIF($B$2:$B25,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B25,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B25,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B25,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -1179,7 +1187,7 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="4"/>
-        <v>h24 python3 -u subapp.py &amp;&gt; h24.out &amp;</v>
+        <v>h24 python3 -u pubapp.py &amp;&gt; h24.out &amp;</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1189,7 +1197,7 @@
       </c>
       <c r="B27" t="str">
         <f>IF(COUNTIF($B$2:$B26,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B26,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B26,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B26,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -1205,7 +1213,7 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="4"/>
-        <v>h25 python3 -u subapp.py &amp;&gt; h25.out &amp;</v>
+        <v>h25 python3 -u pubapp.py &amp;&gt; h25.out &amp;</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1215,7 +1223,7 @@
       </c>
       <c r="B28" t="str">
         <f>IF(COUNTIF($B$2:$B27,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B27,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B27,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B27,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v>subapp.py</v>
+        <v>pubapp.py</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -1231,17 +1239,17 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="4"/>
-        <v>h26 python3 -u subapp.py &amp;&gt; h26.out &amp;</v>
+        <v>h26 python3 -u pubapp.py &amp;&gt; h26.out &amp;</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A29">
+        <f t="shared" si="3"/>
+        <v>27</v>
       </c>
       <c r="B29" t="str">
         <f>IF(COUNTIF($B$2:$B28,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B28,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B28,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B28,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -1253,21 +1261,21 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h27</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>h27 python3 -u pubapp.py &amp;&gt; h27.out &amp;</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A30">
+        <f t="shared" si="3"/>
+        <v>28</v>
       </c>
       <c r="B30" t="str">
         <f>IF(COUNTIF($B$2:$B29,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B29,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B29,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B29,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1279,21 +1287,21 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h28</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ref="F4:F67" si="5">IF(A30="","",IF(B30=$L$1,"h1 ../apache-zookeeper-3.7.0-bin/bin/zkServer.sh&amp; &amp;&amp; zooinspector&amp;",_xlfn.CONCAT(E30," python3 -u ",B30,IF(AND(B30=$G$1,$B$1&gt;0)," -d broker","")," &amp;&gt; ",E30,".out &amp;")))</f>
-        <v/>
+        <f t="shared" ref="F30:F67" si="5">IF(A30="","",IF(B30=$L$1,"h1 ../apache-zookeeper-3.7.0-bin/bin/zkServer.sh&amp; &amp;&amp; zooinspector&amp;",_xlfn.CONCAT(E30," python3 -u ",B30,IF(AND(B30=$G$1,$B$1&gt;0)," -d broker","")," &amp;&gt; ",E30,".out &amp;")))</f>
+        <v>h28 python3 -u pubapp.py &amp;&gt; h28.out &amp;</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A31">
+        <f t="shared" si="3"/>
+        <v>29</v>
       </c>
       <c r="B31" t="str">
         <f>IF(COUNTIF($B$2:$B30,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B30,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B30,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B30,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -1305,21 +1313,21 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h29</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h29 python3 -u pubapp.py &amp;&gt; h29.out &amp;</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A32">
+        <f t="shared" si="3"/>
+        <v>30</v>
       </c>
       <c r="B32" t="str">
         <f>IF(COUNTIF($B$2:$B31,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B31,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B31,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B31,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1331,21 +1339,21 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h30</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h30 python3 -u pubapp.py &amp;&gt; h30.out &amp;</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A33">
+        <f t="shared" si="3"/>
+        <v>31</v>
       </c>
       <c r="B33" t="str">
         <f>IF(COUNTIF($B$2:$B32,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B32,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B32,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B32,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -1357,21 +1365,21 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h31</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h31 python3 -u pubapp.py &amp;&gt; h31.out &amp;</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A34">
+        <f t="shared" si="3"/>
+        <v>32</v>
       </c>
       <c r="B34" t="str">
         <f>IF(COUNTIF($B$2:$B33,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B33,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B33,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B33,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1383,21 +1391,21 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h32</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h32 python3 -u pubapp.py &amp;&gt; h32.out &amp;</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A35">
+        <f t="shared" si="3"/>
+        <v>33</v>
       </c>
       <c r="B35" t="str">
         <f>IF(COUNTIF($B$2:$B34,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B34,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B34,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B34,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -1409,21 +1417,21 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h33</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h33 python3 -u pubapp.py &amp;&gt; h33.out &amp;</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A36">
+        <f t="shared" si="3"/>
+        <v>34</v>
       </c>
       <c r="B36" t="str">
         <f>IF(COUNTIF($B$2:$B35,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B35,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B35,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B35,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -1435,21 +1443,21 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h34</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h34 python3 -u pubapp.py &amp;&gt; h34.out &amp;</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A37">
+        <f t="shared" si="3"/>
+        <v>35</v>
       </c>
       <c r="B37" t="str">
         <f>IF(COUNTIF($B$2:$B36,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B36,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B36,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B36,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -1461,21 +1469,21 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h35</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h35 python3 -u pubapp.py &amp;&gt; h35.out &amp;</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A38">
+        <f t="shared" si="3"/>
+        <v>36</v>
       </c>
       <c r="B38" t="str">
         <f>IF(COUNTIF($B$2:$B37,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B37,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B37,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B37,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -1487,21 +1495,21 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h36</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h36 python3 -u pubapp.py &amp;&gt; h36.out &amp;</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A39">
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="B39" t="str">
         <f>IF(COUNTIF($B$2:$B38,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B38,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B38,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B38,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
@@ -1513,21 +1521,21 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h37</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h37 python3 -u pubapp.py &amp;&gt; h37.out &amp;</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A40">
+        <f t="shared" si="3"/>
+        <v>38</v>
       </c>
       <c r="B40" t="str">
         <f>IF(COUNTIF($B$2:$B39,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B39,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B39,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B39,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -1539,21 +1547,21 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h38</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h38 python3 -u pubapp.py &amp;&gt; h38.out &amp;</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A41">
+        <f t="shared" si="3"/>
+        <v>39</v>
       </c>
       <c r="B41" t="str">
         <f>IF(COUNTIF($B$2:$B40,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B40,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B40,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B40,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
@@ -1565,21 +1573,21 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h39</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h39 python3 -u pubapp.py &amp;&gt; h39.out &amp;</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A42">
+        <f t="shared" si="3"/>
+        <v>40</v>
       </c>
       <c r="B42" t="str">
         <f>IF(COUNTIF($B$2:$B41,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B41,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B41,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B41,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
@@ -1591,21 +1599,21 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h40</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h40 python3 -u pubapp.py &amp;&gt; h40.out &amp;</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A43">
+        <f t="shared" si="3"/>
+        <v>41</v>
       </c>
       <c r="B43" t="str">
         <f>IF(COUNTIF($B$2:$B42,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B42,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B42,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B42,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
@@ -1617,21 +1625,21 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h41</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h41 python3 -u pubapp.py &amp;&gt; h41.out &amp;</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A44">
+        <f t="shared" si="3"/>
+        <v>42</v>
       </c>
       <c r="B44" t="str">
         <f>IF(COUNTIF($B$2:$B43,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B43,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B43,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B43,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
@@ -1643,21 +1651,21 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h42</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h42 python3 -u pubapp.py &amp;&gt; h42.out &amp;</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A45">
+        <f t="shared" si="3"/>
+        <v>43</v>
       </c>
       <c r="B45" t="str">
         <f>IF(COUNTIF($B$2:$B44,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B44,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B44,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B44,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
@@ -1669,21 +1677,21 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h43</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h43 python3 -u pubapp.py &amp;&gt; h43.out &amp;</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A46">
+        <f t="shared" si="3"/>
+        <v>44</v>
       </c>
       <c r="B46" t="str">
         <f>IF(COUNTIF($B$2:$B45,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B45,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B45,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B45,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
@@ -1695,21 +1703,21 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h44</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h44 python3 -u pubapp.py &amp;&gt; h44.out &amp;</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A47">
+        <f t="shared" si="3"/>
+        <v>45</v>
       </c>
       <c r="B47" t="str">
         <f>IF(COUNTIF($B$2:$B46,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B46,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B46,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B46,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
@@ -1721,21 +1729,21 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h45</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h45 python3 -u pubapp.py &amp;&gt; h45.out &amp;</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A48">
+        <f t="shared" si="3"/>
+        <v>46</v>
       </c>
       <c r="B48" t="str">
         <f>IF(COUNTIF($B$2:$B47,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B47,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B47,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B47,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
@@ -1747,21 +1755,21 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h46</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h46 python3 -u pubapp.py &amp;&gt; h46.out &amp;</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A49">
+        <f t="shared" si="3"/>
+        <v>47</v>
       </c>
       <c r="B49" t="str">
         <f>IF(COUNTIF($B$2:$B48,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B48,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B48,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B48,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
@@ -1773,21 +1781,21 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h47</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h47 python3 -u pubapp.py &amp;&gt; h47.out &amp;</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A50">
+        <f t="shared" si="3"/>
+        <v>48</v>
       </c>
       <c r="B50" t="str">
         <f>IF(COUNTIF($B$2:$B49,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B49,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B49,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B49,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
@@ -1799,21 +1807,21 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h48</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h48 python3 -u pubapp.py &amp;&gt; h48.out &amp;</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A51">
+        <f t="shared" si="3"/>
+        <v>49</v>
       </c>
       <c r="B51" t="str">
         <f>IF(COUNTIF($B$2:$B50,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B50,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B50,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B50,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>pubapp.py</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
@@ -1825,21 +1833,21 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h49</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h49 python3 -u pubapp.py &amp;&gt; h49.out &amp;</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A52">
+        <f t="shared" si="3"/>
+        <v>50</v>
       </c>
       <c r="B52" t="str">
         <f>IF(COUNTIF($B$2:$B51,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B51,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B51,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B51,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
@@ -1851,21 +1859,21 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h50</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h50 python3 -u subapp.py &amp;&gt; h50.out &amp;</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A53">
+        <f t="shared" si="3"/>
+        <v>51</v>
       </c>
       <c r="B53" t="str">
         <f>IF(COUNTIF($B$2:$B52,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B52,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B52,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B52,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
@@ -1877,21 +1885,21 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h51</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h51 python3 -u subapp.py &amp;&gt; h51.out &amp;</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A54">
+        <f t="shared" si="3"/>
+        <v>52</v>
       </c>
       <c r="B54" t="str">
         <f>IF(COUNTIF($B$2:$B53,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B53,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B53,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B53,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
@@ -1903,21 +1911,21 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h52</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h52 python3 -u subapp.py &amp;&gt; h52.out &amp;</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A55">
+        <f t="shared" si="3"/>
+        <v>53</v>
       </c>
       <c r="B55" t="str">
         <f>IF(COUNTIF($B$2:$B54,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B54,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B54,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B54,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
@@ -1929,21 +1937,21 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h53</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h53 python3 -u subapp.py &amp;&gt; h53.out &amp;</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A56">
+        <f t="shared" si="3"/>
+        <v>54</v>
       </c>
       <c r="B56" t="str">
         <f>IF(COUNTIF($B$2:$B55,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B55,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B55,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B55,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
@@ -1955,21 +1963,21 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h54</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h54 python3 -u subapp.py &amp;&gt; h54.out &amp;</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A57">
+        <f t="shared" si="3"/>
+        <v>55</v>
       </c>
       <c r="B57" t="str">
         <f>IF(COUNTIF($B$2:$B56,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B56,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B56,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B56,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
@@ -1981,21 +1989,21 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h55</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h55 python3 -u subapp.py &amp;&gt; h55.out &amp;</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A58">
+        <f t="shared" si="3"/>
+        <v>56</v>
       </c>
       <c r="B58" t="str">
         <f>IF(COUNTIF($B$2:$B57,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B57,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B57,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B57,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
@@ -2007,21 +2015,21 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h56</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h56 python3 -u subapp.py &amp;&gt; h56.out &amp;</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A59">
+        <f t="shared" si="3"/>
+        <v>57</v>
       </c>
       <c r="B59" t="str">
         <f>IF(COUNTIF($B$2:$B58,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B58,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B58,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B58,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
@@ -2033,21 +2041,21 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h57</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h57 python3 -u subapp.py &amp;&gt; h57.out &amp;</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A60">
+        <f t="shared" si="3"/>
+        <v>58</v>
       </c>
       <c r="B60" t="str">
         <f>IF(COUNTIF($B$2:$B59,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B59,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B59,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B59,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
@@ -2059,21 +2067,21 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h58</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h58 python3 -u subapp.py &amp;&gt; h58.out &amp;</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A61">
+        <f t="shared" si="3"/>
+        <v>59</v>
       </c>
       <c r="B61" t="str">
         <f>IF(COUNTIF($B$2:$B60,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B60,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B60,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B60,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
@@ -2085,21 +2093,21 @@
       </c>
       <c r="E61" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h59</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h59 python3 -u subapp.py &amp;&gt; h59.out &amp;</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A62">
+        <f t="shared" si="3"/>
+        <v>60</v>
       </c>
       <c r="B62" t="str">
         <f>IF(COUNTIF($B$2:$B61,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B61,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B61,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B61,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
@@ -2111,21 +2119,21 @@
       </c>
       <c r="E62" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h60</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h60 python3 -u subapp.py &amp;&gt; h60.out &amp;</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A63">
+        <f t="shared" si="3"/>
+        <v>61</v>
       </c>
       <c r="B63" t="str">
         <f>IF(COUNTIF($B$2:$B62,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B62,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B62,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B62,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
@@ -2137,21 +2145,21 @@
       </c>
       <c r="E63" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h61</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h61 python3 -u subapp.py &amp;&gt; h61.out &amp;</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A64">
+        <f t="shared" si="3"/>
+        <v>62</v>
       </c>
       <c r="B64" t="str">
         <f>IF(COUNTIF($B$2:$B63,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B63,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B63,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B63,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
@@ -2163,21 +2171,21 @@
       </c>
       <c r="E64" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h62</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h62 python3 -u subapp.py &amp;&gt; h62.out &amp;</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A65">
+        <f t="shared" si="3"/>
+        <v>63</v>
       </c>
       <c r="B65" t="str">
         <f>IF(COUNTIF($B$2:$B64,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B64,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B64,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B64,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
@@ -2189,21 +2197,21 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h63</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h63 python3 -u subapp.py &amp;&gt; h63.out &amp;</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A66">
+        <f t="shared" si="3"/>
+        <v>64</v>
       </c>
       <c r="B66" t="str">
         <f>IF(COUNTIF($B$2:$B65,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B65,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B65,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B65,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
@@ -2215,21 +2223,21 @@
       </c>
       <c r="E66" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>h64</v>
       </c>
       <c r="F66" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h64 python3 -u subapp.py &amp;&gt; h64.out &amp;</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="A67">
+        <f t="shared" si="3"/>
+        <v>65</v>
       </c>
       <c r="B67" t="str">
         <f>IF(COUNTIF($B$2:$B66,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B66,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B66,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B66,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C115" si="6">IF(AND($A66&lt;$J$1*$K$1,ISNUMBER($A67)),CEILING($A67/$K$1,1),"")</f>
@@ -2241,21 +2249,21 @@
       </c>
       <c r="E67" t="str">
         <f t="shared" ref="E67:E105" si="8">IF(AND(ISNUMBER(C67),ISNUMBER(D67)),_xlfn.CONCAT("h",C67,"x",D67),IF(ISNUMBER($A67),_xlfn.CONCAT("h",A67),""))</f>
-        <v/>
+        <v>h65</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>h65 python3 -u subapp.py &amp;&gt; h65.out &amp;</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" t="str">
+      <c r="A68">
         <f t="shared" ref="A68:A131" si="9">IF(OR(A67=$B$1+$D$1+$F$1+$H$1+1,A67=""),"",A67+1)</f>
-        <v/>
+        <v>66</v>
       </c>
       <c r="B68" t="str">
         <f>IF(COUNTIF($B$2:$B67,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B67,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B67,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B67,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="6"/>
@@ -2267,21 +2275,21 @@
       </c>
       <c r="E68" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h66</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" ref="F68:F119" si="10">IF(A68="","",IF(B68=$L$1,"h1 ../apache-zookeeper-3.7.0-bin/bin/zkServer.sh&amp; &amp;&amp; zooinspector&amp;",_xlfn.CONCAT(E68," python3 -u ",B68,IF(AND(B68=$G$1,$B$1&gt;0)," -d broker","")," &amp;&gt; ",E68,".out &amp;")))</f>
-        <v/>
+        <v>h66 python3 -u subapp.py &amp;&gt; h66.out &amp;</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A69">
+        <f t="shared" si="9"/>
+        <v>67</v>
       </c>
       <c r="B69" t="str">
         <f>IF(COUNTIF($B$2:$B68,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B68,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B68,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B68,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="6"/>
@@ -2293,21 +2301,21 @@
       </c>
       <c r="E69" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h67</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h67 python3 -u subapp.py &amp;&gt; h67.out &amp;</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A70">
+        <f t="shared" si="9"/>
+        <v>68</v>
       </c>
       <c r="B70" t="str">
         <f>IF(COUNTIF($B$2:$B69,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B69,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B69,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B69,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="6"/>
@@ -2319,21 +2327,21 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h68</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h68 python3 -u subapp.py &amp;&gt; h68.out &amp;</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A71">
+        <f t="shared" si="9"/>
+        <v>69</v>
       </c>
       <c r="B71" t="str">
         <f>IF(COUNTIF($B$2:$B70,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B70,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B70,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B70,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="6"/>
@@ -2345,21 +2353,21 @@
       </c>
       <c r="E71" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h69</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h69 python3 -u subapp.py &amp;&gt; h69.out &amp;</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A72">
+        <f t="shared" si="9"/>
+        <v>70</v>
       </c>
       <c r="B72" t="str">
         <f>IF(COUNTIF($B$2:$B71,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B71,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B71,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B71,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="6"/>
@@ -2371,21 +2379,21 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h70</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h70 python3 -u subapp.py &amp;&gt; h70.out &amp;</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A73">
+        <f t="shared" si="9"/>
+        <v>71</v>
       </c>
       <c r="B73" t="str">
         <f>IF(COUNTIF($B$2:$B72,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B72,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B72,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B72,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="6"/>
@@ -2397,21 +2405,21 @@
       </c>
       <c r="E73" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h71</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h71 python3 -u subapp.py &amp;&gt; h71.out &amp;</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A74">
+        <f t="shared" si="9"/>
+        <v>72</v>
       </c>
       <c r="B74" t="str">
         <f>IF(COUNTIF($B$2:$B73,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B73,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B73,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B73,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="6"/>
@@ -2423,21 +2431,21 @@
       </c>
       <c r="E74" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h72</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h72 python3 -u subapp.py &amp;&gt; h72.out &amp;</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A75">
+        <f t="shared" si="9"/>
+        <v>73</v>
       </c>
       <c r="B75" t="str">
         <f>IF(COUNTIF($B$2:$B74,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B74,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B74,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B74,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="6"/>
@@ -2449,21 +2457,21 @@
       </c>
       <c r="E75" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h73</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h73 python3 -u subapp.py &amp;&gt; h73.out &amp;</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A76">
+        <f t="shared" si="9"/>
+        <v>74</v>
       </c>
       <c r="B76" t="str">
         <f>IF(COUNTIF($B$2:$B75,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B75,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B75,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B75,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="6"/>
@@ -2475,21 +2483,21 @@
       </c>
       <c r="E76" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h74</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h74 python3 -u subapp.py &amp;&gt; h74.out &amp;</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A77">
+        <f t="shared" si="9"/>
+        <v>75</v>
       </c>
       <c r="B77" t="str">
         <f>IF(COUNTIF($B$2:$B76,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B76,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B76,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B76,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="6"/>
@@ -2501,21 +2509,21 @@
       </c>
       <c r="E77" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h75</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h75 python3 -u subapp.py &amp;&gt; h75.out &amp;</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A78">
+        <f t="shared" si="9"/>
+        <v>76</v>
       </c>
       <c r="B78" t="str">
         <f>IF(COUNTIF($B$2:$B77,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B77,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B77,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B77,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="6"/>
@@ -2527,21 +2535,21 @@
       </c>
       <c r="E78" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h76</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h76 python3 -u subapp.py &amp;&gt; h76.out &amp;</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A79">
+        <f t="shared" si="9"/>
+        <v>77</v>
       </c>
       <c r="B79" t="str">
         <f>IF(COUNTIF($B$2:$B78,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B78,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B78,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B78,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="6"/>
@@ -2553,21 +2561,21 @@
       </c>
       <c r="E79" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h77</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h77 python3 -u subapp.py &amp;&gt; h77.out &amp;</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A80">
+        <f t="shared" si="9"/>
+        <v>78</v>
       </c>
       <c r="B80" t="str">
         <f>IF(COUNTIF($B$2:$B79,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B79,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B79,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B79,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="6"/>
@@ -2579,21 +2587,21 @@
       </c>
       <c r="E80" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h78</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h78 python3 -u subapp.py &amp;&gt; h78.out &amp;</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A81">
+        <f t="shared" si="9"/>
+        <v>79</v>
       </c>
       <c r="B81" t="str">
         <f>IF(COUNTIF($B$2:$B80,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B80,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B80,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B80,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="6"/>
@@ -2605,21 +2613,21 @@
       </c>
       <c r="E81" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h79</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h79 python3 -u subapp.py &amp;&gt; h79.out &amp;</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A82">
+        <f t="shared" si="9"/>
+        <v>80</v>
       </c>
       <c r="B82" t="str">
         <f>IF(COUNTIF($B$2:$B81,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B81,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B81,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B81,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="6"/>
@@ -2631,21 +2639,21 @@
       </c>
       <c r="E82" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h80</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h80 python3 -u subapp.py &amp;&gt; h80.out &amp;</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A83">
+        <f t="shared" si="9"/>
+        <v>81</v>
       </c>
       <c r="B83" t="str">
         <f>IF(COUNTIF($B$2:$B82,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B82,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B82,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B82,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="6"/>
@@ -2657,21 +2665,21 @@
       </c>
       <c r="E83" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h81</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h81 python3 -u subapp.py &amp;&gt; h81.out &amp;</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A84">
+        <f t="shared" si="9"/>
+        <v>82</v>
       </c>
       <c r="B84" t="str">
         <f>IF(COUNTIF($B$2:$B83,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B83,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B83,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B83,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="6"/>
@@ -2683,21 +2691,21 @@
       </c>
       <c r="E84" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h82</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h82 python3 -u subapp.py &amp;&gt; h82.out &amp;</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A85">
+        <f t="shared" si="9"/>
+        <v>83</v>
       </c>
       <c r="B85" t="str">
         <f>IF(COUNTIF($B$2:$B84,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B84,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B84,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B84,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="6"/>
@@ -2709,21 +2717,21 @@
       </c>
       <c r="E85" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h83</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h83 python3 -u subapp.py &amp;&gt; h83.out &amp;</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A86">
+        <f t="shared" si="9"/>
+        <v>84</v>
       </c>
       <c r="B86" t="str">
         <f>IF(COUNTIF($B$2:$B85,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B85,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B85,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B85,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="6"/>
@@ -2735,21 +2743,21 @@
       </c>
       <c r="E86" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h84</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h84 python3 -u subapp.py &amp;&gt; h84.out &amp;</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A87">
+        <f t="shared" si="9"/>
+        <v>85</v>
       </c>
       <c r="B87" t="str">
         <f>IF(COUNTIF($B$2:$B86,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B86,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B86,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B86,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="6"/>
@@ -2761,21 +2769,21 @@
       </c>
       <c r="E87" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h85</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h85 python3 -u subapp.py &amp;&gt; h85.out &amp;</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A88">
+        <f t="shared" si="9"/>
+        <v>86</v>
       </c>
       <c r="B88" t="str">
         <f>IF(COUNTIF($B$2:$B87,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B87,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B87,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B87,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="6"/>
@@ -2787,21 +2795,21 @@
       </c>
       <c r="E88" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h86</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h86 python3 -u subapp.py &amp;&gt; h86.out &amp;</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A89">
+        <f t="shared" si="9"/>
+        <v>87</v>
       </c>
       <c r="B89" t="str">
         <f>IF(COUNTIF($B$2:$B88,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B88,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B88,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B88,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="6"/>
@@ -2813,21 +2821,21 @@
       </c>
       <c r="E89" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h87</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h87 python3 -u subapp.py &amp;&gt; h87.out &amp;</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A90">
+        <f t="shared" si="9"/>
+        <v>88</v>
       </c>
       <c r="B90" t="str">
         <f>IF(COUNTIF($B$2:$B89,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B89,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B89,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B89,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="6"/>
@@ -2839,21 +2847,21 @@
       </c>
       <c r="E90" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h88</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h88 python3 -u subapp.py &amp;&gt; h88.out &amp;</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A91">
+        <f t="shared" si="9"/>
+        <v>89</v>
       </c>
       <c r="B91" t="str">
         <f>IF(COUNTIF($B$2:$B90,$G$1)&lt;$H$1,$G$1,IF(COUNTIF($B$2:$B90,$A$1)&lt;$B$1,$A$1,IF(COUNTIF($B$2:$B90,$C$1)&lt;$D$1,$C$1,IF(COUNTIF($B$2:$B90,$E$1)&lt;$F$1,$E$1,""))))</f>
-        <v/>
+        <v>subapp.py</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="6"/>
@@ -2865,11 +2873,11 @@
       </c>
       <c r="E91" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>h89</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>h89 python3 -u subapp.py &amp;&gt; h89.out &amp;</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -3616,7 +3624,7 @@
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="str">
-        <f t="shared" ref="A132:A141" si="13">IF(OR(A132=$B$1+$D$1+$F$1+$H$1,A132=""),"",A132+1)</f>
+        <f t="shared" ref="A133:A141" si="13">IF(OR(A132=$B$1+$D$1+$F$1+$H$1,A132=""),"",A132+1)</f>
         <v/>
       </c>
     </row>

</xml_diff>